<commit_message>
second commit for further development
</commit_message>
<xml_diff>
--- a/resource/dayr.xlsx
+++ b/resource/dayr.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liujinlc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\workspaces\goPath\src\github.com\dayr-trade-calculator\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="152">
   <si>
     <t>Jam</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -583,6 +583,49 @@
   </si>
   <si>
     <t>Bryansk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lymph</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chelyabinsk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gorenicji (Kiev)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Irkutsk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Krasnoyarsk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magnitogorsk (fitter)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magnitogorsk (trader)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Omsk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rostov-On-Don</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sverdlovsk</t>
+  </si>
+  <si>
+    <t>Sverdlovsk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1143,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X31"/>
+  <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34:T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1190,7 +1233,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="11"/>
       <c r="H2" s="15" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1280,7 +1323,7 @@
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -1508,7 +1551,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="11"/>
       <c r="H8" s="16" t="s">
-        <v>89</v>
+        <v>146</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1516,7 +1559,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="11"/>
       <c r="N8" s="16" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -1828,7 +1871,7 @@
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B14" s="16" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1871,7 +1914,7 @@
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="16" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1879,7 +1922,7 @@
       <c r="L15" s="6"/>
       <c r="M15" s="11"/>
       <c r="N15" s="16" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -2104,7 +2147,7 @@
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B20" s="16" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2415,7 +2458,7 @@
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B27" s="16" t="s">
-        <v>82</v>
+        <v>144</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2423,7 +2466,7 @@
       <c r="F27" s="6"/>
       <c r="G27" s="11"/>
       <c r="H27" s="16" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -2663,6 +2706,31 @@
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
+    </row>
+    <row r="34" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T34" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T35" s="29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T36" s="29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T37" s="29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T38" s="29" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2675,7 +2743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B27"/>
     </sheetView>
   </sheetViews>
@@ -4203,10 +4271,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4226,26 +4294,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C1" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>39</v>
+      <c r="B1" s="29" t="s">
+        <v>17</v>
       </c>
       <c r="K1" s="29" t="s">
         <v>136</v>
@@ -4253,28 +4303,7 @@
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="29" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="K2" s="29" t="s">
         <v>137</v>
@@ -4282,28 +4311,7 @@
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="29" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="K3" s="28" t="s">
         <v>138</v>
@@ -4311,62 +4319,23 @@
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="29" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="K4" s="28" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="29" t="s">
+        <v>6</v>
+      </c>
       <c r="K5" s="28" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="H6" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="K6" s="28" t="s">
         <v>80</v>
@@ -4374,25 +4343,7 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="H7" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="I7" s="29" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="K7" s="28" t="s">
         <v>135</v>
@@ -4400,25 +4351,7 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="K8" s="28" t="s">
         <v>57</v>
@@ -4426,270 +4359,569 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="H9" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="I9" s="29" t="s">
-        <v>125</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="E10" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>43</v>
+      <c r="B10" s="29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="29" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D14" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>104</v>
+      <c r="B14" s="29" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" s="29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B31" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="29" t="s">
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B32" s="29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" s="29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" s="29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" s="29" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" s="29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" s="29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" s="29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" s="29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B48" s="29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" s="29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" s="29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="29" t="s">
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" s="29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" s="29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56" s="29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B57" s="29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B58" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B59" s="29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B60" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B61" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B62" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B63" s="29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B64" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" s="29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" s="29" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" s="29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74" s="29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" s="29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76" s="29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B77" s="29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78" s="29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80" s="29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81" s="29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B83" s="29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B84" s="29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B85" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B86" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B87" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B88" s="29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B89" s="29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B90" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B91" s="29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B92" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B93" s="29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B94" s="29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B95" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B96" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B97" s="29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B98" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B99" s="29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B100" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B101" s="29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B102" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B103" s="29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B104" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B105" s="29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B106" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="G15" s="29" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D16" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="G20" s="29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D21" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="G21" s="29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="G25" s="29" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="G26" s="29" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="29" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="G28" s="29" t="s">
-        <v>121</v>
-      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B107"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B108"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B109"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B110"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B111"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B112"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B113"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B114"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B115"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B116"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B117"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B118"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B119"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B120"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B121"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B122"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B123"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B124"/>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B125"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B126"/>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B127"/>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B128"/>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B129"/>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B130"/>
     </row>
   </sheetData>
-  <sortState ref="K1:K8">
-    <sortCondition ref="K1"/>
+  <sortState ref="B1:B130">
+    <sortCondition ref="B1"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>